<commit_message>
Updated data entering logic
</commit_message>
<xml_diff>
--- a/SkinX-Disease.xlsx
+++ b/SkinX-Disease.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isuruudara/Desktop/SDGP/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C6A8D6-3CB5-3047-8251-ACCDACBE5D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -216,33 +225,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF374151"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -251,7 +265,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -267,51 +281,54 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -501,26 +518,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="29.38"/>
-    <col customWidth="1" min="2" max="2" width="89.38"/>
-    <col customWidth="1" min="3" max="3" width="76.0"/>
-    <col customWidth="1" min="4" max="4" width="146.38"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="89.33203125" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="146.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +576,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" ht="93.0" customHeight="1">
+    <row r="2" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -570,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="112.5" customHeight="1">
+    <row r="3" spans="1:26" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -584,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="121.5" customHeight="1">
+    <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -598,7 +618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="72.75" customHeight="1">
+    <row r="5" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -612,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" ht="68.25" customHeight="1">
+    <row r="6" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -624,7 +644,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" ht="124.5" customHeight="1">
+    <row r="7" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -636,7 +656,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" ht="92.25" customHeight="1">
+    <row r="8" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
@@ -648,7 +668,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" ht="103.5" customHeight="1">
+    <row r="9" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -660,12 +680,12 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
@@ -673,14 +693,14 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -688,7 +708,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -696,6 +716,6 @@
       <c r="C14" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add skin diseaase data to db file
</commit_message>
<xml_diff>
--- a/SkinX-Disease.xlsx
+++ b/SkinX-Disease.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isuruudara/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A585BA7-AB8D-2646-9D8F-950D7D551C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Skin Disease</t>
   </si>
@@ -201,48 +210,153 @@
 Sleep disturbances due to itchiness or discomfort</t>
   </si>
   <si>
-    <t>Ringworm(To be added)</t>
-  </si>
-  <si>
-    <t>Warts Molluscum (To be added)</t>
-  </si>
-  <si>
-    <t>Serorrheic Keratoses (To be added)</t>
-  </si>
-  <si>
     <t>Nail Fungus</t>
+  </si>
+  <si>
+    <t>Eggplant and apple cider vinegar.
+Baking soda and coconut oil paste.
+Black salve or bloodroot.
+Oils: black raspberry seed, frankincense, and myrrh.
+Iodine.
+Vitamin C.</t>
+  </si>
+  <si>
+    <t>Ringworm</t>
+  </si>
+  <si>
+    <t>A mild solution of bleach and water may ease inflammation and itching, as well as killing the bacteria that can cause skin infections when you have eczema. ...
+Add apple cider vinegar to bath water. ...
+Use mild soaps or body cleansers. ...
+Moisturize your skin twice a day. ...
+Apply coconut oil to damp skin once or twice a day.</t>
+  </si>
+  <si>
+    <t>Ringworm often causes a ring-shaped rash that is itchy, scaly and slightly raised. The rings usually start small and then expand outward. Ringworm of the body (tinea corporis) is a rash caused by a fungal infection. It's usually an itchy, circular rash with clearer skin in the middle</t>
+  </si>
+  <si>
+    <t>Itchy skin.
+Ring-shaped rash.
+Red, scaly, cracked skin.
+Hair loss</t>
+  </si>
+  <si>
+    <t>Garlic. - Garlic paste may be used as a topical treatment, although no studies have been conducted on its use. ...
+Soapy water. ...
+Apple cider vinegar. ...
+Aloe vera. ...
+Coconut oil. ...
+Grapefruit seed extract. ...
+Turmeric. ...
+Powdered licorice</t>
+  </si>
+  <si>
+    <t>Warts Molluscum</t>
+  </si>
+  <si>
+    <t>They often have a pearly appearance. They're usually smooth and firm. In most people, the lesions range from about the size of a pinhead to as large as a pencil eraser (2 to 5 millimeters in diameter). They may become itchy, sore, red, and/or swollen.</t>
+  </si>
+  <si>
+    <t>First sign
+The bumps appear on the skin between 2 and 8 weeks after you get the virus that causes this skin infection.
+When the bumps first appear, you usually see ones that are small, firm, pink, flesh-colored, or white. These bumps will likely get bigger.</t>
+  </si>
+  <si>
+    <t>Just apply one cup of cider vinegar to bath water and submerge nightly for 10 minutes or so. Cold compresses can also be applied to itchy or irritated bumps. How can it be prevented? Within reason, try to prevent skin-to-skin contact with someone who has molluscum</t>
+  </si>
+  <si>
+    <t>Serorrheic Keratoses</t>
+  </si>
+  <si>
+    <t>A seborrheic keratosis (seb-o-REE-ik ker-uh-TOE-sis) is a common noncancerous (benign) skin growth. People tend to get more of them as they get older. Seborrheic keratoses are usually brown, black or light tan. The growths (lesions) look waxy or scaly and slightly raised.</t>
+  </si>
+  <si>
+    <t>Be slightly raised from the surrounding skin.
+Be white or light tan in appearance, which may darken to brown or black.
+Have a waxy, pasted-on look.
+Look scaly or like a wart.
+Be well-defined from the surrounding skin.
+Not usually cause pain but may sometimes itch a little.</t>
+  </si>
+  <si>
+    <t>There are no proven home remedies for seborrheic keratoses. Lemon juice or vinegar can irritate the skin, possibly causing the lesion to dry and crumble. However, there is no evidence that this is safe or effective.</t>
+  </si>
+  <si>
+    <t>Nail fungus is a common infection of the nail. It begins as a white or yellow-brown spot under the tip of your fingernail or toenail. As the fungal infection goes deeper, the nail may discolor, thicken and crumble at the edge. Nail fungus can affect several nails</t>
+  </si>
+  <si>
+    <t>Diabetes and think you're developing nail fungus.
+Bleeding around the nails.
+Swelling or pain around the nails.
+Difficulty walking</t>
+  </si>
+  <si>
+    <t>Oils. Some oils contain antifungal, anti-bacterial, and/or antiseptic qualities. ...
+Garlic. Garlic includes strong antifungal properties, making this a top home remedy for treating particular strains of toenail fungus. ...
+Snakeroot Extract. ...
+Baking Soda. ...
+Mentholated Topical Ointment.</t>
+  </si>
+  <si>
+    <t>No home treatment, Immediately meet a doctor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF374151"/>
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -251,7 +365,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -267,51 +381,72 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -501,26 +636,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="29.38"/>
-    <col customWidth="1" min="2" max="2" width="89.38"/>
-    <col customWidth="1" min="3" max="3" width="76.0"/>
-    <col customWidth="1" min="4" max="4" width="146.38"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="89.33203125" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="146.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,146 +696,175 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" ht="93.0" customHeight="1">
+    <row r="2" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="112.5" customHeight="1">
+    <row r="3" spans="1:26" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="121.5" customHeight="1">
+    <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="72.75" customHeight="1">
+    <row r="5" spans="1:26" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" ht="68.25" customHeight="1">
+    <row r="6" spans="1:26" ht="110" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" ht="124.5" customHeight="1">
+      <c r="D6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" ht="92.25" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" ht="103.5" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="D8" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="D9" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="97" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="119" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add the medicine and show it in front end
</commit_message>
<xml_diff>
--- a/SkinX-Disease.xlsx
+++ b/SkinX-Disease.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isuruudara/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isuruudara/Desktop/SDGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A585BA7-AB8D-2646-9D8F-950D7D551C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E78555A-0DA7-514A-A385-E75504D59FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Skin Disease</t>
   </si>
@@ -299,12 +299,85 @@
   <si>
     <t>No home treatment, Immediately meet a doctor</t>
   </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Topical retinoids
+Topical antibiotics
+Isotretinoin
+Benzoyl Peroxide Cream
+Salicylic Acid Cream</t>
+  </si>
+  <si>
+    <t>Topical corticosteroids
+Barrier creams
+Emollients
+Oral Antihistamines
+Systemic Immunosuppressants</t>
+  </si>
+  <si>
+    <t>Biologic Drugs
+Methotrexate
+Cyclosporine
+Clobetasol
+Calcipotriene
+Coal Tar</t>
+  </si>
+  <si>
+    <t>Imiquimod
+5-Fluorouracil
+Photodynamic Therapy
+Vismodegib
+Sonidegib</t>
+  </si>
+  <si>
+    <t>Chemotherapy
+Immunotherapy
+Efudex
+Aldara
+Zyclara</t>
+  </si>
+  <si>
+    <t>Topical corticosteroid
+Topical emollients
+Immunotherapy
+Chemotherapy</t>
+  </si>
+  <si>
+    <t>antihistamines
+cetirizine
+diphenhydramie
+Benadryl</t>
+  </si>
+  <si>
+    <t>Griseofulvin (Grifulvin V, Gris-PEG)
+Terbinafine.
+Itraconazole (Onmel, Sporanox)
+Fluconazole (Diflucan)</t>
+  </si>
+  <si>
+    <t>iodine 
+salicylic acid
+potassium hydroxide
+tretinoin cantharidin</t>
+  </si>
+  <si>
+    <t>Eskata</t>
+  </si>
+  <si>
+    <t>efinaconazole
+tavaborole</t>
+  </si>
+  <si>
+    <t>Melanocytic nevi can be surgically removed for cosmetic considerations or because of concern regarding the biological potential of a lesion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -315,22 +388,26 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF374151"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -358,6 +435,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial (Body)"/>
     </font>
   </fonts>
   <fills count="4">
@@ -392,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -415,7 +497,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -428,6 +509,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -658,6 +741,7 @@
     <col min="2" max="2" width="89.33203125" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
     <col min="4" max="4" width="146.33203125" customWidth="1"/>
+    <col min="5" max="5" width="74.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
@@ -673,7 +757,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -709,6 +795,9 @@
       <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -723,6 +812,9 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -737,6 +829,9 @@
       <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -751,6 +846,9 @@
       <c r="D5" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="E5" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="110" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -765,6 +863,9 @@
       <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="E6" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -779,9 +880,12 @@
       <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="E7" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -790,12 +894,15 @@
       <c r="C8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="E8" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -804,64 +911,79 @@
       <c r="C9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="E9" s="13" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="E10" s="13" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="E11" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="97" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="E12" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="119" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>49</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Updated Backend in backend branch
</commit_message>
<xml_diff>
--- a/SkinX-Disease.xlsx
+++ b/SkinX-Disease.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isuruudara/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isuruudara/Desktop/SDGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A585BA7-AB8D-2646-9D8F-950D7D551C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E78555A-0DA7-514A-A385-E75504D59FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Skin Disease</t>
   </si>
@@ -299,12 +299,85 @@
   <si>
     <t>No home treatment, Immediately meet a doctor</t>
   </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Topical retinoids
+Topical antibiotics
+Isotretinoin
+Benzoyl Peroxide Cream
+Salicylic Acid Cream</t>
+  </si>
+  <si>
+    <t>Topical corticosteroids
+Barrier creams
+Emollients
+Oral Antihistamines
+Systemic Immunosuppressants</t>
+  </si>
+  <si>
+    <t>Biologic Drugs
+Methotrexate
+Cyclosporine
+Clobetasol
+Calcipotriene
+Coal Tar</t>
+  </si>
+  <si>
+    <t>Imiquimod
+5-Fluorouracil
+Photodynamic Therapy
+Vismodegib
+Sonidegib</t>
+  </si>
+  <si>
+    <t>Chemotherapy
+Immunotherapy
+Efudex
+Aldara
+Zyclara</t>
+  </si>
+  <si>
+    <t>Topical corticosteroid
+Topical emollients
+Immunotherapy
+Chemotherapy</t>
+  </si>
+  <si>
+    <t>antihistamines
+cetirizine
+diphenhydramie
+Benadryl</t>
+  </si>
+  <si>
+    <t>Griseofulvin (Grifulvin V, Gris-PEG)
+Terbinafine.
+Itraconazole (Onmel, Sporanox)
+Fluconazole (Diflucan)</t>
+  </si>
+  <si>
+    <t>iodine 
+salicylic acid
+potassium hydroxide
+tretinoin cantharidin</t>
+  </si>
+  <si>
+    <t>Eskata</t>
+  </si>
+  <si>
+    <t>efinaconazole
+tavaborole</t>
+  </si>
+  <si>
+    <t>Melanocytic nevi can be surgically removed for cosmetic considerations or because of concern regarding the biological potential of a lesion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -315,22 +388,26 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF374151"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -358,6 +435,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial (Body)"/>
     </font>
   </fonts>
   <fills count="4">
@@ -392,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -415,7 +497,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -428,6 +509,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -658,6 +741,7 @@
     <col min="2" max="2" width="89.33203125" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
     <col min="4" max="4" width="146.33203125" customWidth="1"/>
+    <col min="5" max="5" width="74.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
@@ -673,7 +757,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -709,6 +795,9 @@
       <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -723,6 +812,9 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -737,6 +829,9 @@
       <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -751,6 +846,9 @@
       <c r="D5" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="E5" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="110" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -765,6 +863,9 @@
       <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="E6" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -779,9 +880,12 @@
       <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="E7" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -790,12 +894,15 @@
       <c r="C8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="E8" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -804,64 +911,79 @@
       <c r="C9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="E9" s="13" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="E10" s="13" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="E11" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="97" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="E12" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="119" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>49</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>